<commit_message>
Assigned TABULA Heating and hot water techs
According to the TABULA webtool heating types. See updated documentation for main assumptions. Used Gas boiler + solar thermal flatplate collectors for heating when required or solar thermal only for hot water (because hot water cannot be combined).
</commit_message>
<xml_diff>
--- a/cea/databases/DE/assemblies/SUPPLY.xlsx
+++ b/cea/databases/DE/assemblies/SUPPLY.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zshi/Documents/GitHub/CityEnergyAnalyst/cea/databases/DE/assemblies/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ge38yoz\CityEnergyAnalyst\cea\databases\DE\assemblies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B57E32-63E6-3B47-99A6-CDD4A36F7BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86F2992C-8A81-4345-84B3-9A8BAD2CE946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5740" yWindow="1480" windowWidth="41340" windowHeight="24520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="0" windowWidth="19190" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HEATING" sheetId="1" r:id="rId1"/>
@@ -46,19 +46,11 @@
   <commentList>
     <comment ref="A33" authorId="0" shapeId="0" xr:uid="{B4F5AB91-6F7C-483D-A592-89102691FFFB}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     All values + 15% of vertailverluste not included in th original factors. In order to trasnform from useful to final energy
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -73,19 +65,11 @@
   <commentList>
     <comment ref="A33" authorId="0" shapeId="0" xr:uid="{003A11DB-1C47-4897-99B3-6450868F736D}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     All values + 15% of vertailverluste not included in th original factors. In order to trasnform from useful to final energy
 </t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -93,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="177">
   <si>
     <t>Description</t>
   </si>
@@ -600,6 +584,30 @@
   </si>
   <si>
     <t>BO7</t>
+  </si>
+  <si>
+    <t>condensing boiler + solar thermal collector</t>
+  </si>
+  <si>
+    <t>SUPPLY_HEATING_AS36</t>
+  </si>
+  <si>
+    <t>SC1</t>
+  </si>
+  <si>
+    <t>solar thermal collector</t>
+  </si>
+  <si>
+    <t>SUPPLY_HEATING_AS37</t>
+  </si>
+  <si>
+    <t>SOLAR</t>
+  </si>
+  <si>
+    <t>Flatplate collector</t>
+  </si>
+  <si>
+    <t>SUPPLY_HOTWATER_AS36</t>
   </si>
 </sst>
 </file>
@@ -734,7 +742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -845,6 +853,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3C3C3C"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3C3C3C"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -852,7 +891,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -935,11 +974,38 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1256,27 +1322,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21:C37"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="22" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="77.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6328125" customWidth="1"/>
+    <col min="11" max="11" width="12.6328125" customWidth="1"/>
+    <col min="13" max="13" width="77.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +1383,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -1358,7 +1424,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -1399,7 +1465,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -1440,7 +1506,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -1481,7 +1547,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1522,7 +1588,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -1563,7 +1629,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -1604,7 +1670,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -1645,7 +1711,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -1686,7 +1752,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1727,7 +1793,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -1768,7 +1834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -1809,7 +1875,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -1850,7 +1916,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -1891,7 +1957,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -1932,7 +1998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -1973,7 +2039,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -2014,7 +2080,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -2055,7 +2121,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
@@ -2096,7 +2162,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
@@ -2137,7 +2203,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>58</v>
       </c>
@@ -2178,7 +2244,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>60</v>
       </c>
@@ -2219,7 +2285,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -2260,7 +2326,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -2301,7 +2367,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -2342,7 +2408,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>70</v>
       </c>
@@ -2383,7 +2449,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -2424,7 +2490,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -2465,7 +2531,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
@@ -2506,7 +2572,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
@@ -2547,7 +2613,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -2588,7 +2654,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
@@ -2629,7 +2695,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>88</v>
       </c>
@@ -2670,7 +2736,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -2713,7 +2779,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" s="23" t="s">
         <v>150</v>
       </c>
@@ -2755,7 +2821,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" ht="26" x14ac:dyDescent="0.35">
       <c r="A37" s="23" t="s">
         <v>149</v>
       </c>
@@ -2795,6 +2861,89 @@
       </c>
       <c r="M37" s="24" t="s">
         <v>153</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C38" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>157</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+      <c r="I38" s="8">
+        <f>142+600</f>
+        <v>742</v>
+      </c>
+      <c r="J38" s="6">
+        <v>20</v>
+      </c>
+      <c r="K38" s="6">
+        <v>3</v>
+      </c>
+      <c r="L38" s="6">
+        <v>5</v>
+      </c>
+      <c r="M38" s="30" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" s="31" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C39" s="33" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="F39" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="G39" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="H39" s="8">
+        <v>1</v>
+      </c>
+      <c r="I39">
+        <v>600</v>
+      </c>
+      <c r="J39" s="36">
+        <v>20</v>
+      </c>
+      <c r="K39" s="36">
+        <v>3</v>
+      </c>
+      <c r="L39" s="36">
+        <v>5</v>
+      </c>
+      <c r="M39" s="37" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -2807,26 +2956,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J37"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35:J37"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="51.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="77.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="10" max="10" width="77.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2858,7 +3007,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -2890,7 +3039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>99</v>
       </c>
@@ -2922,7 +3071,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
@@ -2954,7 +3103,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -2986,7 +3135,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -3018,7 +3167,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
@@ -3050,7 +3199,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
@@ -3082,7 +3231,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -3114,7 +3263,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -3146,7 +3295,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -3178,7 +3327,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>35</v>
       </c>
@@ -3210,7 +3359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>38</v>
       </c>
@@ -3242,7 +3391,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
@@ -3274,7 +3423,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -3306,7 +3455,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>44</v>
       </c>
@@ -3338,7 +3487,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>46</v>
       </c>
@@ -3370,7 +3519,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>48</v>
       </c>
@@ -3402,7 +3551,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>50</v>
       </c>
@@ -3434,7 +3583,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>52</v>
       </c>
@@ -3466,7 +3615,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
@@ -3498,7 +3647,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="12" t="s">
         <v>58</v>
       </c>
@@ -3530,7 +3679,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="12" t="s">
         <v>60</v>
       </c>
@@ -3562,7 +3711,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>62</v>
       </c>
@@ -3594,7 +3743,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>66</v>
       </c>
@@ -3626,7 +3775,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>68</v>
       </c>
@@ -3658,7 +3807,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>70</v>
       </c>
@@ -3690,7 +3839,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>72</v>
       </c>
@@ -3722,7 +3871,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>74</v>
       </c>
@@ -3754,7 +3903,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>76</v>
       </c>
@@ -3786,7 +3935,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>79</v>
       </c>
@@ -3818,7 +3967,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
@@ -3850,7 +3999,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>85</v>
       </c>
@@ -3882,7 +4031,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>88</v>
       </c>
@@ -3914,7 +4063,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>91</v>
       </c>
@@ -3947,7 +4096,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>94</v>
       </c>
@@ -3979,7 +4128,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>96</v>
       </c>
@@ -4009,6 +4158,38 @@
       </c>
       <c r="J37" s="21" t="s">
         <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A38" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="B38" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C38" s="35" t="s">
+        <v>174</v>
+      </c>
+      <c r="D38" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="E38" s="38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="38">
+        <v>600</v>
+      </c>
+      <c r="G38" s="36">
+        <v>20</v>
+      </c>
+      <c r="H38" s="36">
+        <v>3</v>
+      </c>
+      <c r="I38" s="36">
+        <v>5</v>
+      </c>
+      <c r="J38" s="37" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -4023,24 +4204,24 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="21.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="14" max="14" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="21.1796875" customWidth="1"/>
+    <col min="7" max="7" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.6328125" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="14" max="14" width="51.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4084,7 +4265,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4128,7 +4309,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>76</v>
       </c>
@@ -4172,7 +4353,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
@@ -4216,7 +4397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>140</v>
       </c>
@@ -4260,7 +4441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>142</v>
       </c>
@@ -4315,23 +4496,23 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="92.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="10" max="10" width="70.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="92.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="12.6328125" customWidth="1"/>
+    <col min="10" max="10" width="70.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4363,7 +4544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -4395,7 +4576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>147</v>
       </c>

</xml_diff>